<commit_message>
Editing user manual: N cycling
</commit_message>
<xml_diff>
--- a/tables/23-sediment_biogeochemistry/UserManual.xlsx
+++ b/tables/23-sediment_biogeochemistry/UserManual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00074264\AED Dropbox\AED_Coorong_db\5_reporting\CDM Manual\DanDrafts\aed-science\tables\23-sediment_biogeochemistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65ABB5DA-6D8C-4483-95C0-A5A8FA15958F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5829FD0-BB85-45F8-BC2D-EDCAB0B1352F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31485" yWindow="-2970" windowWidth="26235" windowHeight="16440" firstSheet="1" activeTab="6" xr2:uid="{24890297-503A-4F29-AEBF-DF10B16371ED}"/>
   </bookViews>
@@ -20,9 +20,7 @@
     <sheet name="OMChem" sheetId="7" r:id="rId5"/>
     <sheet name="SecondChem" sheetId="8" r:id="rId6"/>
     <sheet name="OMApproach" sheetId="9" r:id="rId7"/>
-    <sheet name="Sheet9" sheetId="10" r:id="rId8"/>
-    <sheet name="OMApproach (2)" sheetId="11" r:id="rId9"/>
-    <sheet name="Test" sheetId="12" r:id="rId10"/>
+    <sheet name="NRates" sheetId="13" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_Ref386302068" localSheetId="3">OMModel!#REF!</definedName>
@@ -51,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="163">
   <si>
     <t>Same for all zones</t>
   </si>
@@ -4617,35 +4615,6 @@
       </rPr>
       <t>In</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">\(\displaystyle
-\
-\frac {TEA}{TEA + K_{TEA} }\)
-\
-\
-</t>
-  </si>
-  <si>
-    <t>\(\displaystyle
-\
-\frac {K_{In}} {TEA + K_{In} }\)
-\
-\</t>
-  </si>
-  <si>
-    <t>\(\displaystyle
-\
-\frac {K_{In}}{TEA+K_{In} } \)
-\
-\</t>
-  </si>
-  <si>
-    <t>\(\displaystyle
-\
-\frac {TEA}{TEA+K_{TEA} } / \Sigma Lim \)
-\
-\</t>
   </si>
   <si>
     <t>\
@@ -4711,12 +4680,85 @@
 \
 \</t>
   </si>
+  <si>
+    <t>Denitratation</t>
+  </si>
+  <si>
+    <t>Nitrous denitritation</t>
+  </si>
+  <si>
+    <t>DNRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denitrousation </t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>\
+\(\displaystyle
+\
+\ R_{Denitratation} = k_{OM} OM \frac {NO_3^-} {NO_3^- + K_{NO3} } \frac {K_{O2}^1} {O_2 + K_{O2}^1} \frac {K_{N2O}} {N_2O + K_{N2O}}   \)
+\
+\</t>
+  </si>
+  <si>
+    <t>Denitritation</t>
+  </si>
+  <si>
+    <t>\
+\(\displaystyle
+\
+\ R_{Denitritation} = k_{OM} OM \frac {K_{O2}^3} {O_2 + K_{O2}^3 } \frac {K_{N2O}} {N_2O + K_{NO2} }    \)
+\
+\</t>
+  </si>
+  <si>
+    <t>\
+\(\displaystyle
+\
+\ R_{Nitrous denitritation} = \frac {1} {2} R_{Denitritation} \frac {NO_2^- } {NO_2^- + K_{NO2} }    \)
+\
+\</t>
+  </si>
+  <si>
+    <t>\
+\(\displaystyle
+\
+\ R_{DNRA} = R_{Denitritation} \frac {K_{NO2} } {NO_2^- + K_{NO2} }    \)
+\
+\</t>
+  </si>
+  <si>
+    <t>\
+\(\displaystyle
+\
+\ R_{Denitrousation} = k_{OM} OM  \frac {K_{N2O} } {K_{N2O}^6 +O_2 }    \)
+\
+\</t>
+  </si>
+  <si>
+    <t>Ammonium release</t>
+  </si>
+  <si>
+    <t>\
+\(\displaystyle
+\
+\ R_{Ammonium release} = k_{OM} OM \times
+\\
+(R_{Denitratation} +  R_{Denitritation} +  R_{Denitrousation}) \times 
+\\
+ \frac {N } {C }    \)
+\
+\</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4853,8 +4895,16 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4867,8 +4917,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -4990,17 +5046,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -5141,20 +5186,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5725,101 +5768,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1EE45D8-67C5-4E51-A390-600014CFF6F8}">
-  <dimension ref="B1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="47" customWidth="1"/>
-    <col min="4" max="4" width="43.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="41" t="s">
-        <v>140</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="42">
-        <v>1</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="42">
-        <v>2</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="46">
-        <v>3</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="47" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="14"/>
-    </row>
-    <row r="7" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="14"/>
-    </row>
-    <row r="8" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="14"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BBA0FB1-7A19-4ECF-8FF5-02D3A0E6D618}">
   <dimension ref="A1:C9"/>
@@ -5922,15 +5870,35 @@
   <dimension ref="B2:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27:L37"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="8" spans="2:4" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="42">
+        <v>3</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="46"/>
     </row>
     <row r="27" spans="12:12" ht="24" x14ac:dyDescent="0.25">
       <c r="L27" s="9" t="s">
@@ -6570,10 +6538,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB823B2-7167-4378-A45D-8972DC675CE8}">
-  <dimension ref="B1:D6"/>
+  <dimension ref="B1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6600,10 +6568,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="114.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6611,31 +6579,11 @@
         <v>2</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="42">
-        <v>3</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="145.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="42" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="49"/>
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6644,90 +6592,73 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A72CCB72-B98E-4A77-A95C-BEEC16023647}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404188C7-A26D-4F82-A2ED-9697F94CBCFE}">
+  <dimension ref="B1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32542531-B1D0-45E8-A2E2-27735870BFCC}">
-  <dimension ref="B2:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="34"/>
-    <col min="2" max="2" width="8.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" style="34" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="34"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="114" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="9" t="s">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>48</v>
+    </row>
+    <row r="2" spans="2:3" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Internal links; Case studies
</commit_message>
<xml_diff>
--- a/tables/23-sediment_biogeochemistry/UserManual.xlsx
+++ b/tables/23-sediment_biogeochemistry/UserManual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00074264\AED Dropbox\AED_Coorong_db\5_reporting\CDM Manual\DanDrafts\aed-science\tables\23-sediment_biogeochemistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF65A14-4577-4570-B78F-63AC372E8AD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688EF3AF-E1E2-4D7A-9C7E-2B196862EC0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60135" yWindow="-1335" windowWidth="26385" windowHeight="16440" firstSheet="3" activeTab="11" xr2:uid="{24890297-503A-4F29-AEBF-DF10B16371ED}"/>
+    <workbookView xWindow="60135" yWindow="-1335" windowWidth="26385" windowHeight="16440" firstSheet="12" activeTab="23" xr2:uid="{24890297-503A-4F29-AEBF-DF10B16371ED}"/>
   </bookViews>
   <sheets>
     <sheet name="BoundaryInitial" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,14 @@
     <sheet name="ads" sheetId="21" r:id="rId16"/>
     <sheet name="MAG" sheetId="22" r:id="rId17"/>
     <sheet name="MPBG" sheetId="23" r:id="rId18"/>
+    <sheet name="VCW1" sheetId="25" r:id="rId19"/>
+    <sheet name="UAE" sheetId="26" r:id="rId20"/>
+    <sheet name="UAE2" sheetId="27" r:id="rId21"/>
+    <sheet name="UAE3" sheetId="28" r:id="rId22"/>
+    <sheet name="UAE4" sheetId="29" r:id="rId23"/>
+    <sheet name="UAE5" sheetId="30" r:id="rId24"/>
+    <sheet name="UAE6" sheetId="31" r:id="rId25"/>
+    <sheet name="UAE7" sheetId="32" r:id="rId26"/>
   </sheets>
   <definedNames>
     <definedName name="_Ref386302068" localSheetId="4">OMModel!#REF!</definedName>
@@ -59,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="589">
   <si>
     <t>Same for all zones</t>
   </si>
@@ -5600,12 +5608,965 @@
   <si>
     <t>4Fe^2+^ + O_2 + 8HCO_3^- + 2H_2O $\rightarrow$  4Fe(OH)3A + 8CO_2</t>
   </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Biodiffusion constant</t>
+  </si>
+  <si>
+    <t>4 to 36</t>
+  </si>
+  <si>
+    <t>Depth of biodiffusion decrease</t>
+  </si>
+  <si>
+    <t>20 to 30</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>Bioirrigation coefficient</t>
+  </si>
+  <si>
+    <t>100 to 300</t>
+  </si>
+  <si>
+    <t>0.02 to 0.54</t>
+  </si>
+  <si>
+    <t>N:C ratio</t>
+  </si>
+  <si>
+    <t>9.6 to 32</t>
+  </si>
+  <si>
+    <t>N atoms:106 C atoms</t>
+  </si>
+  <si>
+    <t>P:C ratio</t>
+  </si>
+  <si>
+    <t>0.7 to 1.55</t>
+  </si>
+  <si>
+    <t>P atoms:106 C atoms</t>
+  </si>
+  <si>
+    <t>Aerobic oxidation limitation concentration</t>
+  </si>
+  <si>
+    <t>Denitrification limitation concentration</t>
+  </si>
+  <si>
+    <t>1.1 to 1.7</t>
+  </si>
+  <si>
+    <t>Siderite dissolution constant</t>
+  </si>
+  <si>
+    <t>*DB~0~*</t>
+  </si>
+  <si>
+    <t>*x~b~*</t>
+  </si>
+  <si>
+    <t>*α~0~*</t>
+  </si>
+  <si>
+    <t>*x~irrig~*</t>
+  </si>
+  <si>
+    <t>*y~Lab~*</t>
+  </si>
+  <si>
+    <t>*z~Lab~*</t>
+  </si>
+  <si>
+    <t>*K~TEAO2~*</t>
+  </si>
+  <si>
+    <t>*~KTEANO3~*</t>
+  </si>
+  <si>
+    <t>*k~NH4ads~*</t>
+  </si>
+  <si>
+    <t>*k~FeOx~*</t>
+  </si>
+  <si>
+    <r>
+      <t>1×10^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-2^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to 3×10^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-2^</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4×10^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-3^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to 6×10^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>^</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5×10^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to 5×10^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4^</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.5×10^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-5^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to 2.5×10^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-3^</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>y^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>^</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>cm^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> y^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1^</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>y^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1^</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>mmol L^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>^</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>mmol L^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> y^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>^</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*NH~</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4~^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>+^*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> adsorption coefficient</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Kinetic rate constant for aerobic oxidation of *Fe^</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>^*</t>
+    </r>
+  </si>
+  <si>
+    <t>*k~Siddis~*</t>
+  </si>
+  <si>
+    <t>Modelled variable</t>
+  </si>
+  <si>
+    <r>
+      <t>2.4 x 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.5 x 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.3 x 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.8 x 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.2 x 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.6 x 10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>O~2~</t>
+  </si>
+  <si>
+    <t>NH~4~^+^</t>
+  </si>
+  <si>
+    <t>NO~3~^-^</t>
+  </si>
+  <si>
+    <t>PO~4~^3-^</t>
+  </si>
+  <si>
+    <t>SO~4~^2-^</t>
+  </si>
+  <si>
+    <t>HCO~3~^-^</t>
+  </si>
+  <si>
+    <t>POM~R~</t>
+  </si>
+  <si>
+    <t>Field measurement (mg L^-1^)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modelled boundary (mmol L^-1^) </t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>Aquaculture</t>
+  </si>
+  <si>
+    <t>Immediate post-aquaculture</t>
+  </si>
+  <si>
+    <t>Recovery</t>
+  </si>
+  <si>
+    <t>Aquaculture periods (period of active cage aquaculture)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 years </t>
+  </si>
+  <si>
+    <t>1 year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 years </t>
+  </si>
+  <si>
+    <t>10 years</t>
+  </si>
+  <si>
+    <t>3 years</t>
+  </si>
+  <si>
+    <t>2 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 years </t>
+  </si>
+  <si>
+    <t>5 years</t>
+  </si>
+  <si>
+    <t>6 years</t>
+  </si>
+  <si>
+    <t>Time step</t>
+  </si>
+  <si>
+    <t>5 days</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>0.5 days</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>Fish waste fluxes (mmol C m^-2^ y^-1^)</t>
+  </si>
+  <si>
+    <t>1×10^2^, 5×10^2^</t>
+  </si>
+  <si>
+    <t>1×10^3^, 5×10^3^, 1×10^4^</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5×10^4^, 1×10^5^, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5×10^5^, 1×10^6^, </t>
+  </si>
+  <si>
+    <t>5×10^6^</t>
+  </si>
+  <si>
+    <t>Time period / Time step</t>
+  </si>
+  <si>
+    <t>NO3</t>
+  </si>
+  <si>
+    <t>PO4</t>
+  </si>
+  <si>
+    <t>NH4</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>OM Flux</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>×10^</t>
+    </r>
+  </si>
+  <si>
+    <t>5×10^</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>1×10^7^</t>
+  </si>
+  <si>
+    <t>1×10^2^</t>
+  </si>
+  <si>
+    <t>OM Flux upper range</t>
+  </si>
+  <si>
+    <t>1×10^7^ to 5×10^6^</t>
+  </si>
+  <si>
+    <t>5×10^6^ to 1×10^6^</t>
+  </si>
+  <si>
+    <t>1×10^6^ to 5×10^5^</t>
+  </si>
+  <si>
+    <t>5×10^5^ to 1×10^5^</t>
+  </si>
+  <si>
+    <t>1×10^5^ to 5×10^4^</t>
+  </si>
+  <si>
+    <t>5×10^4^ to 1×10^4^</t>
+  </si>
+  <si>
+    <t>1×10^4^ to 5×10^3^</t>
+  </si>
+  <si>
+    <t>5×10^3^ to 1×10^3^</t>
+  </si>
+  <si>
+    <t>1×10^3^ to 5×10^2^</t>
+  </si>
+  <si>
+    <t>5×10^2^ to 1×10^2^</t>
+  </si>
+  <si>
+    <t>1 Year</t>
+  </si>
+  <si>
+    <t>2 Years</t>
+  </si>
+  <si>
+    <t>3 Years</t>
+  </si>
+  <si>
+    <t>5 Years</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>&lt; </t>
+  </si>
+  <si>
+    <t>&lt;1 year recovery</t>
+  </si>
+  <si>
+    <t>2 year recovery</t>
+  </si>
+  <si>
+    <t>3 year recovery</t>
+  </si>
+  <si>
+    <t>4 year recovery</t>
+  </si>
+  <si>
+    <t>5 year recovery</t>
+  </si>
+  <si>
+    <t>6 year recovery</t>
+  </si>
+  <si>
+    <t>7 year recovery</t>
+  </si>
+  <si>
+    <t>&gt; 8 year recovery</t>
+  </si>
+  <si>
+    <t>0 to 202000</t>
+  </si>
+  <si>
+    <t>0 to 174000</t>
+  </si>
+  <si>
+    <t>0 to 145000</t>
+  </si>
+  <si>
+    <t>0 to 88100</t>
+  </si>
+  <si>
+    <t>202000 to 480000</t>
+  </si>
+  <si>
+    <t>174000 to 403000</t>
+  </si>
+  <si>
+    <t>145000 to 327000</t>
+  </si>
+  <si>
+    <t>88100 to 173000</t>
+  </si>
+  <si>
+    <t>480000 to 758000</t>
+  </si>
+  <si>
+    <t>403000 to 633000</t>
+  </si>
+  <si>
+    <t>327000 to 508000</t>
+  </si>
+  <si>
+    <t>173000 to 258000</t>
+  </si>
+  <si>
+    <t>758000 to 1040000</t>
+  </si>
+  <si>
+    <t>633000 to 863000</t>
+  </si>
+  <si>
+    <t>508000 to 690000</t>
+  </si>
+  <si>
+    <t>258000 to 343000</t>
+  </si>
+  <si>
+    <t>1040000 to 1310000</t>
+  </si>
+  <si>
+    <t>863000 to 1090000</t>
+  </si>
+  <si>
+    <t>690000 to 871000</t>
+  </si>
+  <si>
+    <t>343000 to 428000</t>
+  </si>
+  <si>
+    <t>1310000 to 1590000</t>
+  </si>
+  <si>
+    <t>1090000 to 1320000</t>
+  </si>
+  <si>
+    <t>871000 to 1050000</t>
+  </si>
+  <si>
+    <t>428000 to 513000</t>
+  </si>
+  <si>
+    <t>1590000 to 1870000</t>
+  </si>
+  <si>
+    <t>1320000 to 1550000</t>
+  </si>
+  <si>
+    <t>1050000 to 1230000</t>
+  </si>
+  <si>
+    <t>513000 to 598000</t>
+  </si>
+  <si>
+    <t>1870000</t>
+  </si>
+  <si>
+    <t>1550000</t>
+  </si>
+  <si>
+    <t>1230000</t>
+  </si>
+  <si>
+    <t>598000</t>
+  </si>
+  <si>
+    <t>Zone of High Impact</t>
+  </si>
+  <si>
+    <t>Zone of Medium-High Impact</t>
+  </si>
+  <si>
+    <t>Zone of Medium Impact</t>
+  </si>
+  <si>
+    <t>Zone of Influence</t>
+  </si>
+  <si>
+    <t>6300 to 78600</t>
+  </si>
+  <si>
+    <t>6200 to 63000</t>
+  </si>
+  <si>
+    <t>6100 to 47300</t>
+  </si>
+  <si>
+    <t>6000 to 45100</t>
+  </si>
+  <si>
+    <t>1400 to 6300</t>
+  </si>
+  <si>
+    <t>1350 to 6200</t>
+  </si>
+  <si>
+    <t>1300 to 6100</t>
+  </si>
+  <si>
+    <t>1300 to 6000</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>Recovery time</t>
+  </si>
+  <si>
+    <r>
+      <t>Table 5: Depositional thresholds (F</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color rgb="FF44546A"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OM</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF44546A"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) for 4 impact zone settings, summarised for 4 aquaculture operation periods.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Table 4: Depositional thresholds (F</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="9"/>
+        <color rgb="FF44546A"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OM</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF44546A"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) for recovery time estimation, summarised for 4 aquaculture operation periods.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5785,8 +6746,90 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="subscript"/>
+      <sz val="9"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5847,8 +6890,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -5974,11 +7041,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6192,6 +7301,185 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="32" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="32" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="32" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="32" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="32" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="32" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="32" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="32" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="32" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7139,7 +8427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B560C3-603A-4072-964D-8AC36A7F1082}">
   <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -8578,7 +9866,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8837,6 +10125,204 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FAB4B4-8799-48FC-8A76-89433647002B}">
+  <dimension ref="B2:L13"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="58.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="79" t="s">
+        <v>421</v>
+      </c>
+      <c r="C2" s="79" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="79" t="s">
+        <v>422</v>
+      </c>
+      <c r="E2" s="79" t="s">
+        <v>423</v>
+      </c>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+    </row>
+    <row r="3" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="87" t="s">
+        <v>442</v>
+      </c>
+      <c r="C3" s="91" t="s">
+        <v>424</v>
+      </c>
+      <c r="D3" s="91" t="s">
+        <v>425</v>
+      </c>
+      <c r="E3" s="88" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="87" t="s">
+        <v>443</v>
+      </c>
+      <c r="C4" s="91" t="s">
+        <v>426</v>
+      </c>
+      <c r="D4" s="91" t="s">
+        <v>427</v>
+      </c>
+      <c r="E4" s="88" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="87" t="s">
+        <v>444</v>
+      </c>
+      <c r="C5" s="91" t="s">
+        <v>429</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>430</v>
+      </c>
+      <c r="E5" s="88" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="87" t="s">
+        <v>445</v>
+      </c>
+      <c r="C6" s="91" t="s">
+        <v>429</v>
+      </c>
+      <c r="D6" s="91" t="s">
+        <v>431</v>
+      </c>
+      <c r="E6" s="88" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="87" t="s">
+        <v>446</v>
+      </c>
+      <c r="C7" s="91" t="s">
+        <v>432</v>
+      </c>
+      <c r="D7" s="91" t="s">
+        <v>433</v>
+      </c>
+      <c r="E7" s="88" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="87" t="s">
+        <v>447</v>
+      </c>
+      <c r="C8" s="91" t="s">
+        <v>435</v>
+      </c>
+      <c r="D8" s="91" t="s">
+        <v>436</v>
+      </c>
+      <c r="E8" s="88" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="87" t="s">
+        <v>448</v>
+      </c>
+      <c r="C9" s="91" t="s">
+        <v>438</v>
+      </c>
+      <c r="D9" s="91" t="s">
+        <v>452</v>
+      </c>
+      <c r="E9" s="88" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="87" t="s">
+        <v>449</v>
+      </c>
+      <c r="C10" s="91" t="s">
+        <v>439</v>
+      </c>
+      <c r="D10" s="91" t="s">
+        <v>453</v>
+      </c>
+      <c r="E10" s="88" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="87" t="s">
+        <v>450</v>
+      </c>
+      <c r="C11" s="91" t="s">
+        <v>461</v>
+      </c>
+      <c r="D11" s="91" t="s">
+        <v>440</v>
+      </c>
+      <c r="E11" s="88" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="87" t="s">
+        <v>451</v>
+      </c>
+      <c r="C12" s="91" t="s">
+        <v>462</v>
+      </c>
+      <c r="D12" s="91" t="s">
+        <v>454</v>
+      </c>
+      <c r="E12" s="88" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="36" t="s">
+        <v>463</v>
+      </c>
+      <c r="C13" s="90" t="s">
+        <v>441</v>
+      </c>
+      <c r="D13" s="90" t="s">
+        <v>455</v>
+      </c>
+      <c r="E13" s="89" t="s">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BBA0FB1-7A19-4ECF-8FF5-02D3A0E6D618}">
   <dimension ref="A1:M41"/>
@@ -9262,6 +10748,2420 @@
       </c>
       <c r="J41" t="s">
         <v>394</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5638044B-CB4C-4C94-A755-7C200927062F}">
+  <dimension ref="A2:F21"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.140625" style="92" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="92" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" style="92" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="79" t="s">
+        <v>464</v>
+      </c>
+      <c r="C2" s="79" t="s">
+        <v>478</v>
+      </c>
+      <c r="D2" s="79" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="93" t="s">
+        <v>471</v>
+      </c>
+      <c r="C3" s="93">
+        <v>7.6</v>
+      </c>
+      <c r="D3" s="93" t="s">
+        <v>465</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="93" t="s">
+        <v>472</v>
+      </c>
+      <c r="C4" s="93">
+        <v>0</v>
+      </c>
+      <c r="D4" s="93">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="93" t="s">
+        <v>473</v>
+      </c>
+      <c r="C5" s="93">
+        <v>0.22</v>
+      </c>
+      <c r="D5" s="93" t="s">
+        <v>466</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="93" t="s">
+        <v>474</v>
+      </c>
+      <c r="C6" s="93">
+        <v>0</v>
+      </c>
+      <c r="D6" s="93">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="93" t="s">
+        <v>475</v>
+      </c>
+      <c r="C7" s="93">
+        <v>3163</v>
+      </c>
+      <c r="D7" s="93" t="s">
+        <v>467</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="93" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" s="93">
+        <v>0</v>
+      </c>
+      <c r="D8" s="93">
+        <v>0</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="93" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" s="93">
+        <v>0</v>
+      </c>
+      <c r="D9" s="93">
+        <v>0</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="93" t="s">
+        <v>476</v>
+      </c>
+      <c r="C10" s="93">
+        <v>109</v>
+      </c>
+      <c r="D10" s="93" t="s">
+        <v>468</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="93" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" s="93">
+        <v>25</v>
+      </c>
+      <c r="D11" s="93" t="s">
+        <v>469</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="93" t="s">
+        <v>477</v>
+      </c>
+      <c r="C12" s="93">
+        <v>1.86</v>
+      </c>
+      <c r="D12" s="93" t="s">
+        <v>470</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="94"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="94"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79383B76-50C0-490F-AC19-3FE2C2CA6837}">
+  <dimension ref="B2:G10"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.7109375" style="92" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" style="92" customWidth="1"/>
+    <col min="4" max="7" width="22.28515625" style="92" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B2" s="108" t="s">
+        <v>499</v>
+      </c>
+      <c r="C2" s="79" t="s">
+        <v>505</v>
+      </c>
+      <c r="D2" s="79" t="s">
+        <v>480</v>
+      </c>
+      <c r="E2" s="79" t="s">
+        <v>481</v>
+      </c>
+      <c r="F2" s="79" t="s">
+        <v>482</v>
+      </c>
+      <c r="G2" s="79" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="106" t="s">
+        <v>484</v>
+      </c>
+      <c r="D3" s="101" t="s">
+        <v>485</v>
+      </c>
+      <c r="E3" s="101" t="s">
+        <v>486</v>
+      </c>
+      <c r="F3" s="101" t="s">
+        <v>487</v>
+      </c>
+      <c r="G3" s="101" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="106"/>
+      <c r="D4" s="101" t="s">
+        <v>488</v>
+      </c>
+      <c r="E4" s="101" t="s">
+        <v>489</v>
+      </c>
+      <c r="F4" s="101" t="s">
+        <v>490</v>
+      </c>
+      <c r="G4" s="101" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="107"/>
+      <c r="D5" s="102" t="s">
+        <v>488</v>
+      </c>
+      <c r="E5" s="102" t="s">
+        <v>492</v>
+      </c>
+      <c r="F5" s="102" t="s">
+        <v>490</v>
+      </c>
+      <c r="G5" s="102" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="100" t="s">
+        <v>500</v>
+      </c>
+      <c r="C6" s="105" t="s">
+        <v>494</v>
+      </c>
+      <c r="D6" s="95" t="s">
+        <v>495</v>
+      </c>
+      <c r="E6" s="96" t="s">
+        <v>495</v>
+      </c>
+      <c r="F6" s="96" t="s">
+        <v>495</v>
+      </c>
+      <c r="G6" s="96" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="97" t="s">
+        <v>501</v>
+      </c>
+      <c r="C7" s="103"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="97" t="s">
+        <v>502</v>
+      </c>
+      <c r="C8" s="103"/>
+      <c r="D8" s="102" t="s">
+        <v>495</v>
+      </c>
+      <c r="E8" s="102" t="s">
+        <v>496</v>
+      </c>
+      <c r="F8" s="102" t="s">
+        <v>495</v>
+      </c>
+      <c r="G8" s="102" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="100" t="s">
+        <v>503</v>
+      </c>
+      <c r="C9" s="103"/>
+      <c r="D9" s="101" t="s">
+        <v>495</v>
+      </c>
+      <c r="E9" s="101" t="s">
+        <v>497</v>
+      </c>
+      <c r="F9" s="101" t="s">
+        <v>497</v>
+      </c>
+      <c r="G9" s="101" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="97" t="s">
+        <v>504</v>
+      </c>
+      <c r="C10" s="104"/>
+      <c r="D10" s="102" t="s">
+        <v>495</v>
+      </c>
+      <c r="E10" s="102" t="s">
+        <v>498</v>
+      </c>
+      <c r="F10" s="102" t="s">
+        <v>498</v>
+      </c>
+      <c r="G10" s="102" t="s">
+        <v>495</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63589976-2265-419F-872C-FD2246847E9E}">
+  <dimension ref="A1:P20"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="110" t="s">
+        <v>510</v>
+      </c>
+      <c r="C2" s="110" t="s">
+        <v>510</v>
+      </c>
+      <c r="D2" s="110" t="s">
+        <v>506</v>
+      </c>
+      <c r="E2" s="110" t="s">
+        <v>507</v>
+      </c>
+      <c r="F2" s="110" t="s">
+        <v>508</v>
+      </c>
+      <c r="G2" s="110" t="s">
+        <v>509</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="C3" s="109">
+        <v>10000000</v>
+      </c>
+      <c r="D3" s="112">
+        <v>178</v>
+      </c>
+      <c r="E3" s="112">
+        <v>-753000</v>
+      </c>
+      <c r="F3" s="112">
+        <v>-1530000</v>
+      </c>
+      <c r="G3" s="112">
+        <v>12000</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I3" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13">
+        <f>LOG10(C3)</f>
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>513</v>
+      </c>
+      <c r="N3" t="str">
+        <f>H3&amp;K3&amp;L3</f>
+        <v>1×10^7^</v>
+      </c>
+      <c r="O3" t="str">
+        <f>N3</f>
+        <v>1×10^7^</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="109">
+        <f>C3</f>
+        <v>10000000</v>
+      </c>
+      <c r="C4" s="109">
+        <v>5000000</v>
+      </c>
+      <c r="D4" s="112">
+        <v>172</v>
+      </c>
+      <c r="E4" s="112">
+        <v>-564000</v>
+      </c>
+      <c r="F4" s="112">
+        <v>-1150000</v>
+      </c>
+      <c r="G4" s="112">
+        <v>11900</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I4" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="J4" s="13">
+        <f>LOG10(B4)</f>
+        <v>7</v>
+      </c>
+      <c r="K4" s="13">
+        <f>LOG10(C4/5)</f>
+        <v>6</v>
+      </c>
+      <c r="L4" t="s">
+        <v>513</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" ref="M4" si="0">H4&amp;J4&amp;L4</f>
+        <v>1×10^7^</v>
+      </c>
+      <c r="N4" t="str">
+        <f>I4&amp;K4&amp;L4</f>
+        <v>5×10^6^</v>
+      </c>
+      <c r="O4" t="str">
+        <f>M4&amp;" to "&amp;N4</f>
+        <v>1×10^7^ to 5×10^6^</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="109">
+        <f>C4</f>
+        <v>5000000</v>
+      </c>
+      <c r="C5" s="109">
+        <v>1000000</v>
+      </c>
+      <c r="D5" s="112">
+        <v>163</v>
+      </c>
+      <c r="E5" s="112">
+        <v>-226000</v>
+      </c>
+      <c r="F5" s="112">
+        <v>-458000</v>
+      </c>
+      <c r="G5" s="112">
+        <v>11800</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I5" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="J5" s="13">
+        <f>LOG10(B5/5)</f>
+        <v>6</v>
+      </c>
+      <c r="K5" s="13">
+        <f t="shared" ref="K5:K15" si="1">LOG10(C5)</f>
+        <v>6</v>
+      </c>
+      <c r="L5" t="s">
+        <v>513</v>
+      </c>
+      <c r="M5" t="str">
+        <f>I5&amp;J5&amp;L5</f>
+        <v>5×10^6^</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" ref="N5" si="2">H5&amp;K5&amp;L5</f>
+        <v>1×10^6^</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" ref="O5:O13" si="3">M5&amp;" to "&amp;N5</f>
+        <v>5×10^6^ to 1×10^6^</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="109">
+        <f>C5</f>
+        <v>1000000</v>
+      </c>
+      <c r="C6" s="109">
+        <f>C5/2</f>
+        <v>500000</v>
+      </c>
+      <c r="D6" s="112">
+        <v>158</v>
+      </c>
+      <c r="E6" s="112">
+        <v>-56500</v>
+      </c>
+      <c r="F6" s="112">
+        <v>-115000</v>
+      </c>
+      <c r="G6" s="112">
+        <v>11700</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I6" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="J6" s="13">
+        <f t="shared" ref="J6:J14" si="4">LOG10(B6)</f>
+        <v>6</v>
+      </c>
+      <c r="K6" s="13">
+        <f t="shared" ref="K6:K15" si="5">LOG10(C6/5)</f>
+        <v>5</v>
+      </c>
+      <c r="L6" t="s">
+        <v>513</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" ref="M6" si="6">H6&amp;J6&amp;L6</f>
+        <v>1×10^6^</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" ref="N6" si="7">I6&amp;K6&amp;L6</f>
+        <v>5×10^5^</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="3"/>
+        <v>1×10^6^ to 5×10^5^</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="109">
+        <f>C6</f>
+        <v>500000</v>
+      </c>
+      <c r="C7" s="109">
+        <f>C6/5</f>
+        <v>100000</v>
+      </c>
+      <c r="D7" s="112">
+        <v>102</v>
+      </c>
+      <c r="E7" s="112">
+        <v>-22600</v>
+      </c>
+      <c r="F7" s="112">
+        <v>-46100</v>
+      </c>
+      <c r="G7" s="112">
+        <v>9310</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I7" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="J7" s="13">
+        <f t="shared" ref="J7:J14" si="8">LOG10(B7/5)</f>
+        <v>5</v>
+      </c>
+      <c r="K7" s="13">
+        <f t="shared" ref="K7:K15" si="9">LOG10(C7)</f>
+        <v>5</v>
+      </c>
+      <c r="L7" t="s">
+        <v>513</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" ref="M7" si="10">I7&amp;J7&amp;L7</f>
+        <v>5×10^5^</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" ref="N7" si="11">H7&amp;K7&amp;L7</f>
+        <v>1×10^5^</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="3"/>
+        <v>5×10^5^ to 1×10^5^</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="109">
+        <f>C7</f>
+        <v>100000</v>
+      </c>
+      <c r="C8" s="109">
+        <f t="shared" ref="C8:C13" si="12">C7/2</f>
+        <v>50000</v>
+      </c>
+      <c r="D8" s="112">
+        <v>28</v>
+      </c>
+      <c r="E8" s="112">
+        <v>-5710</v>
+      </c>
+      <c r="F8" s="112">
+        <v>-11700</v>
+      </c>
+      <c r="G8" s="112">
+        <v>6000</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I8" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="J8" s="13">
+        <f t="shared" ref="J8:J14" si="13">LOG10(B8)</f>
+        <v>5</v>
+      </c>
+      <c r="K8" s="13">
+        <f t="shared" ref="K8:K15" si="14">LOG10(C8/5)</f>
+        <v>4</v>
+      </c>
+      <c r="L8" t="s">
+        <v>513</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" ref="M8" si="15">H8&amp;J8&amp;L8</f>
+        <v>1×10^5^</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" ref="N8" si="16">I8&amp;K8&amp;L8</f>
+        <v>5×10^4^</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="3"/>
+        <v>1×10^5^ to 5×10^4^</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="109">
+        <f>C8</f>
+        <v>50000</v>
+      </c>
+      <c r="C9" s="109">
+        <f t="shared" ref="C9:C13" si="17">C8/5</f>
+        <v>10000</v>
+      </c>
+      <c r="D9" s="112">
+        <v>-10.9</v>
+      </c>
+      <c r="E9" s="112">
+        <v>-2320</v>
+      </c>
+      <c r="F9" s="112">
+        <v>-4730</v>
+      </c>
+      <c r="G9" s="112">
+        <v>3840</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I9" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="J9" s="13">
+        <f t="shared" ref="J9:J14" si="18">LOG10(B9/5)</f>
+        <v>4</v>
+      </c>
+      <c r="K9" s="13">
+        <f t="shared" ref="K9:K15" si="19">LOG10(C9)</f>
+        <v>4</v>
+      </c>
+      <c r="L9" t="s">
+        <v>513</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" ref="M9" si="20">I9&amp;J9&amp;L9</f>
+        <v>5×10^4^</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" ref="N9" si="21">H9&amp;K9&amp;L9</f>
+        <v>1×10^4^</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="3"/>
+        <v>5×10^4^ to 1×10^4^</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="109">
+        <f>C9</f>
+        <v>10000</v>
+      </c>
+      <c r="C10" s="109">
+        <f t="shared" ref="C10:C13" si="22">C9/2</f>
+        <v>5000</v>
+      </c>
+      <c r="D10" s="112">
+        <v>-38.9</v>
+      </c>
+      <c r="E10" s="112">
+        <v>-628</v>
+      </c>
+      <c r="F10" s="112">
+        <v>-1250</v>
+      </c>
+      <c r="G10" s="112">
+        <v>2220</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I10" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="J10" s="13">
+        <f t="shared" ref="J10:J14" si="23">LOG10(B10)</f>
+        <v>4</v>
+      </c>
+      <c r="K10" s="13">
+        <f t="shared" ref="K10:K15" si="24">LOG10(C10/5)</f>
+        <v>3</v>
+      </c>
+      <c r="L10" t="s">
+        <v>513</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" ref="M10" si="25">H10&amp;J10&amp;L10</f>
+        <v>1×10^4^</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" ref="N10" si="26">I10&amp;K10&amp;L10</f>
+        <v>5×10^3^</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="3"/>
+        <v>1×10^4^ to 5×10^3^</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="109">
+        <f>C10</f>
+        <v>5000</v>
+      </c>
+      <c r="C11" s="109">
+        <f t="shared" ref="C11:C13" si="27">C10/5</f>
+        <v>1000</v>
+      </c>
+      <c r="D11" s="112">
+        <v>-56.1</v>
+      </c>
+      <c r="E11" s="112">
+        <v>-289</v>
+      </c>
+      <c r="F11" s="112">
+        <v>-528</v>
+      </c>
+      <c r="G11" s="112">
+        <v>1410</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I11" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="J11" s="13">
+        <f t="shared" ref="J11:J14" si="28">LOG10(B11/5)</f>
+        <v>3</v>
+      </c>
+      <c r="K11" s="13">
+        <f t="shared" ref="K11:K15" si="29">LOG10(C11)</f>
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>513</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" ref="M11" si="30">I11&amp;J11&amp;L11</f>
+        <v>5×10^3^</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" ref="N11" si="31">H11&amp;K11&amp;L11</f>
+        <v>1×10^3^</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="3"/>
+        <v>5×10^3^ to 1×10^3^</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="109">
+        <f>C11</f>
+        <v>1000</v>
+      </c>
+      <c r="C12" s="109">
+        <f t="shared" ref="C12:C13" si="32">C11/2</f>
+        <v>500</v>
+      </c>
+      <c r="D12" s="112">
+        <v>-68.099999999999994</v>
+      </c>
+      <c r="E12" s="112">
+        <v>-120</v>
+      </c>
+      <c r="F12" s="112">
+        <v>-158</v>
+      </c>
+      <c r="G12" s="112">
+        <v>827</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I12" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="J12" s="13">
+        <f t="shared" ref="J12:J14" si="33">LOG10(B12)</f>
+        <v>3</v>
+      </c>
+      <c r="K12" s="13">
+        <f t="shared" ref="K12:K15" si="34">LOG10(C12/5)</f>
+        <v>2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>513</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" ref="M12" si="35">H12&amp;J12&amp;L12</f>
+        <v>1×10^3^</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" ref="N12" si="36">I12&amp;K12&amp;L12</f>
+        <v>5×10^2^</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="3"/>
+        <v>1×10^3^ to 5×10^2^</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="109">
+        <f>C12</f>
+        <v>500</v>
+      </c>
+      <c r="C13" s="109">
+        <f t="shared" ref="C13" si="37">C12/5</f>
+        <v>100</v>
+      </c>
+      <c r="D13" s="112">
+        <v>-66.900000000000006</v>
+      </c>
+      <c r="E13" s="112">
+        <v>-86.1</v>
+      </c>
+      <c r="F13" s="112">
+        <v>-83.5</v>
+      </c>
+      <c r="G13" s="112">
+        <v>604</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I13" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="J13" s="13">
+        <f t="shared" ref="J13:J14" si="38">LOG10(B13/5)</f>
+        <v>2</v>
+      </c>
+      <c r="K13" s="13">
+        <f t="shared" ref="K13:K15" si="39">LOG10(C13)</f>
+        <v>2</v>
+      </c>
+      <c r="L13" t="s">
+        <v>513</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" ref="M13" si="40">I13&amp;J13&amp;L13</f>
+        <v>5×10^2^</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" ref="N13" si="41">H13&amp;K13&amp;L13</f>
+        <v>1×10^2^</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="3"/>
+        <v>5×10^2^ to 1×10^2^</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="109">
+        <f>C13</f>
+        <v>100</v>
+      </c>
+      <c r="C14" s="109"/>
+      <c r="D14" s="112">
+        <v>-64.2</v>
+      </c>
+      <c r="E14" s="112">
+        <v>-70.900000000000006</v>
+      </c>
+      <c r="F14" s="112">
+        <v>-46.1</v>
+      </c>
+      <c r="G14" s="112">
+        <v>460</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="I14" s="111" t="s">
+        <v>512</v>
+      </c>
+      <c r="J14" s="13">
+        <f t="shared" ref="J14" si="42">LOG10(B14)</f>
+        <v>2</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" t="s">
+        <v>513</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" ref="M14" si="43">H14&amp;J14&amp;L14</f>
+        <v>1×10^2^</v>
+      </c>
+      <c r="O14" t="str">
+        <f>M14</f>
+        <v>1×10^2^</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="M15" t="str">
+        <f t="shared" ref="M15" si="44">I15&amp;J15&amp;L15</f>
+        <v/>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" ref="N15" si="45">H15&amp;K15&amp;L15</f>
+        <v/>
+      </c>
+      <c r="O15" s="109"/>
+      <c r="P15" s="109"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="O16" s="109"/>
+      <c r="P16" s="109"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD67E78-D613-46E1-844C-AD6CD38E1719}">
+  <dimension ref="B2:F14"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="110" t="s">
+        <v>516</v>
+      </c>
+      <c r="C2" s="110" t="s">
+        <v>473</v>
+      </c>
+      <c r="D2" s="110" t="s">
+        <v>474</v>
+      </c>
+      <c r="E2" s="110" t="s">
+        <v>472</v>
+      </c>
+      <c r="F2" s="110" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>514</v>
+      </c>
+      <c r="C3" s="112">
+        <v>178</v>
+      </c>
+      <c r="D3" s="112">
+        <v>-753000</v>
+      </c>
+      <c r="E3" s="112">
+        <v>-1530000</v>
+      </c>
+      <c r="F3" s="112">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>517</v>
+      </c>
+      <c r="C4" s="112">
+        <v>172</v>
+      </c>
+      <c r="D4" s="112">
+        <v>-564000</v>
+      </c>
+      <c r="E4" s="112">
+        <v>-1150000</v>
+      </c>
+      <c r="F4" s="112">
+        <v>11900</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>518</v>
+      </c>
+      <c r="C5" s="112">
+        <v>163</v>
+      </c>
+      <c r="D5" s="112">
+        <v>-226000</v>
+      </c>
+      <c r="E5" s="112">
+        <v>-458000</v>
+      </c>
+      <c r="F5" s="112">
+        <v>11800</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>519</v>
+      </c>
+      <c r="C6" s="112">
+        <v>158</v>
+      </c>
+      <c r="D6" s="112">
+        <v>-56500</v>
+      </c>
+      <c r="E6" s="112">
+        <v>-115000</v>
+      </c>
+      <c r="F6" s="112">
+        <v>11700</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>520</v>
+      </c>
+      <c r="C7" s="112">
+        <v>102</v>
+      </c>
+      <c r="D7" s="112">
+        <v>-22600</v>
+      </c>
+      <c r="E7" s="112">
+        <v>-46100</v>
+      </c>
+      <c r="F7" s="112">
+        <v>9310</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>521</v>
+      </c>
+      <c r="C8" s="112">
+        <v>28</v>
+      </c>
+      <c r="D8" s="112">
+        <v>-5710</v>
+      </c>
+      <c r="E8" s="112">
+        <v>-11700</v>
+      </c>
+      <c r="F8" s="112">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>522</v>
+      </c>
+      <c r="C9" s="112">
+        <v>-10.9</v>
+      </c>
+      <c r="D9" s="112">
+        <v>-2320</v>
+      </c>
+      <c r="E9" s="112">
+        <v>-4730</v>
+      </c>
+      <c r="F9" s="112">
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>523</v>
+      </c>
+      <c r="C10" s="112">
+        <v>-38.9</v>
+      </c>
+      <c r="D10" s="112">
+        <v>-628</v>
+      </c>
+      <c r="E10" s="112">
+        <v>-1250</v>
+      </c>
+      <c r="F10" s="112">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>524</v>
+      </c>
+      <c r="C11" s="112">
+        <v>-56.1</v>
+      </c>
+      <c r="D11" s="112">
+        <v>-289</v>
+      </c>
+      <c r="E11" s="112">
+        <v>-528</v>
+      </c>
+      <c r="F11" s="112">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>525</v>
+      </c>
+      <c r="C12" s="112">
+        <v>-68.099999999999994</v>
+      </c>
+      <c r="D12" s="112">
+        <v>-120</v>
+      </c>
+      <c r="E12" s="112">
+        <v>-158</v>
+      </c>
+      <c r="F12" s="112">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>526</v>
+      </c>
+      <c r="C13" s="112">
+        <v>-66.900000000000006</v>
+      </c>
+      <c r="D13" s="112">
+        <v>-86.1</v>
+      </c>
+      <c r="E13" s="112">
+        <v>-83.5</v>
+      </c>
+      <c r="F13" s="112">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>515</v>
+      </c>
+      <c r="C14" s="112">
+        <v>-64.2</v>
+      </c>
+      <c r="D14" s="112">
+        <v>-70.900000000000006</v>
+      </c>
+      <c r="E14" s="112">
+        <v>-46.1</v>
+      </c>
+      <c r="F14" s="112">
+        <v>460</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7495890C-77D0-4EFC-B806-50C2928C6692}">
+  <dimension ref="B2:V25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C2" s="126" t="s">
+        <v>527</v>
+      </c>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126" t="s">
+        <v>528</v>
+      </c>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126" t="s">
+        <v>529</v>
+      </c>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126" t="s">
+        <v>530</v>
+      </c>
+      <c r="J2" s="126"/>
+      <c r="O2" s="113" t="s">
+        <v>527</v>
+      </c>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113" t="s">
+        <v>528</v>
+      </c>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113" t="s">
+        <v>529</v>
+      </c>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113" t="s">
+        <v>530</v>
+      </c>
+      <c r="V2" s="113"/>
+    </row>
+    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="114" t="s">
+        <v>531</v>
+      </c>
+      <c r="D3" s="114" t="s">
+        <v>532</v>
+      </c>
+      <c r="E3" s="114" t="s">
+        <v>531</v>
+      </c>
+      <c r="F3" s="114" t="s">
+        <v>532</v>
+      </c>
+      <c r="G3" s="114" t="s">
+        <v>531</v>
+      </c>
+      <c r="H3" s="114" t="s">
+        <v>532</v>
+      </c>
+      <c r="I3" s="114" t="s">
+        <v>531</v>
+      </c>
+      <c r="J3" s="114" t="s">
+        <v>532</v>
+      </c>
+      <c r="O3" s="114" t="s">
+        <v>531</v>
+      </c>
+      <c r="P3" s="114" t="s">
+        <v>532</v>
+      </c>
+      <c r="Q3" s="114" t="s">
+        <v>531</v>
+      </c>
+      <c r="R3" s="114" t="s">
+        <v>532</v>
+      </c>
+      <c r="S3" s="114" t="s">
+        <v>531</v>
+      </c>
+      <c r="T3" s="114" t="s">
+        <v>532</v>
+      </c>
+      <c r="U3" s="114" t="s">
+        <v>531</v>
+      </c>
+      <c r="V3" s="114" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="115" t="s">
+        <v>533</v>
+      </c>
+      <c r="C4" s="127">
+        <v>0</v>
+      </c>
+      <c r="D4" s="128">
+        <v>202000</v>
+      </c>
+      <c r="E4" s="129">
+        <v>0</v>
+      </c>
+      <c r="F4" s="129">
+        <v>174000</v>
+      </c>
+      <c r="G4" s="130">
+        <v>0</v>
+      </c>
+      <c r="H4" s="130">
+        <v>145000</v>
+      </c>
+      <c r="I4" s="131">
+        <v>0</v>
+      </c>
+      <c r="J4" s="131">
+        <v>88100</v>
+      </c>
+      <c r="N4" s="115" t="s">
+        <v>573</v>
+      </c>
+      <c r="O4" s="116">
+        <v>78600</v>
+      </c>
+      <c r="P4" s="141"/>
+      <c r="Q4" s="117">
+        <v>63000</v>
+      </c>
+      <c r="R4" s="142"/>
+      <c r="S4" s="118">
+        <v>47300</v>
+      </c>
+      <c r="T4" s="143"/>
+      <c r="U4" s="119">
+        <v>45100</v>
+      </c>
+      <c r="V4" s="144"/>
+    </row>
+    <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="120" t="s">
+        <v>534</v>
+      </c>
+      <c r="C5" s="132">
+        <v>202000</v>
+      </c>
+      <c r="D5" s="133">
+        <v>480000</v>
+      </c>
+      <c r="E5" s="134">
+        <v>174000</v>
+      </c>
+      <c r="F5" s="134">
+        <v>403000</v>
+      </c>
+      <c r="G5" s="135">
+        <v>145000</v>
+      </c>
+      <c r="H5" s="135">
+        <v>327000</v>
+      </c>
+      <c r="I5" s="136">
+        <v>88100</v>
+      </c>
+      <c r="J5" s="136">
+        <v>173000</v>
+      </c>
+      <c r="N5" s="120" t="s">
+        <v>574</v>
+      </c>
+      <c r="O5" s="121">
+        <v>6300</v>
+      </c>
+      <c r="P5" s="122">
+        <v>78600</v>
+      </c>
+      <c r="Q5" s="123">
+        <v>6200</v>
+      </c>
+      <c r="R5" s="123">
+        <v>63000</v>
+      </c>
+      <c r="S5" s="124">
+        <v>6100</v>
+      </c>
+      <c r="T5" s="124">
+        <v>47300</v>
+      </c>
+      <c r="U5" s="125">
+        <v>6000</v>
+      </c>
+      <c r="V5" s="125">
+        <v>45100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="120" t="s">
+        <v>535</v>
+      </c>
+      <c r="C6" s="132">
+        <v>480000</v>
+      </c>
+      <c r="D6" s="133">
+        <v>758000</v>
+      </c>
+      <c r="E6" s="134">
+        <v>403000</v>
+      </c>
+      <c r="F6" s="134">
+        <v>633000</v>
+      </c>
+      <c r="G6" s="135">
+        <v>327000</v>
+      </c>
+      <c r="H6" s="135">
+        <v>508000</v>
+      </c>
+      <c r="I6" s="136">
+        <v>173000</v>
+      </c>
+      <c r="J6" s="136">
+        <v>258000</v>
+      </c>
+      <c r="N6" s="120" t="s">
+        <v>575</v>
+      </c>
+      <c r="O6" s="121">
+        <v>1400</v>
+      </c>
+      <c r="P6" s="122">
+        <v>6300</v>
+      </c>
+      <c r="Q6" s="123">
+        <v>1350</v>
+      </c>
+      <c r="R6" s="123">
+        <v>6200</v>
+      </c>
+      <c r="S6" s="124">
+        <v>1300</v>
+      </c>
+      <c r="T6" s="124">
+        <v>6100</v>
+      </c>
+      <c r="U6" s="125">
+        <v>1300</v>
+      </c>
+      <c r="V6" s="125">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="120" t="s">
+        <v>536</v>
+      </c>
+      <c r="C7" s="132">
+        <v>758000</v>
+      </c>
+      <c r="D7" s="133">
+        <v>1040000</v>
+      </c>
+      <c r="E7" s="134">
+        <v>633000</v>
+      </c>
+      <c r="F7" s="134">
+        <v>863000</v>
+      </c>
+      <c r="G7" s="135">
+        <v>508000</v>
+      </c>
+      <c r="H7" s="135">
+        <v>690000</v>
+      </c>
+      <c r="I7" s="136">
+        <v>258000</v>
+      </c>
+      <c r="J7" s="136">
+        <v>343000</v>
+      </c>
+      <c r="N7" s="120" t="s">
+        <v>576</v>
+      </c>
+      <c r="O7" s="145">
+        <v>0</v>
+      </c>
+      <c r="P7" s="122">
+        <v>1400</v>
+      </c>
+      <c r="Q7" s="146">
+        <v>0</v>
+      </c>
+      <c r="R7" s="123">
+        <v>1350</v>
+      </c>
+      <c r="S7" s="147">
+        <v>0</v>
+      </c>
+      <c r="T7" s="124">
+        <v>1300</v>
+      </c>
+      <c r="U7" s="148">
+        <v>0</v>
+      </c>
+      <c r="V7" s="125">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="120" t="s">
+        <v>537</v>
+      </c>
+      <c r="C8" s="132">
+        <v>1040000</v>
+      </c>
+      <c r="D8" s="133">
+        <v>1310000</v>
+      </c>
+      <c r="E8" s="134">
+        <v>863000</v>
+      </c>
+      <c r="F8" s="134">
+        <v>1090000</v>
+      </c>
+      <c r="G8" s="135">
+        <v>690000</v>
+      </c>
+      <c r="H8" s="135">
+        <v>871000</v>
+      </c>
+      <c r="I8" s="136">
+        <v>343000</v>
+      </c>
+      <c r="J8" s="136">
+        <v>428000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="120" t="s">
+        <v>538</v>
+      </c>
+      <c r="C9" s="132">
+        <v>1310000</v>
+      </c>
+      <c r="D9" s="133">
+        <v>1590000</v>
+      </c>
+      <c r="E9" s="134">
+        <v>1090000</v>
+      </c>
+      <c r="F9" s="134">
+        <v>1320000</v>
+      </c>
+      <c r="G9" s="135">
+        <v>871000</v>
+      </c>
+      <c r="H9" s="135">
+        <v>1050000</v>
+      </c>
+      <c r="I9" s="136">
+        <v>428000</v>
+      </c>
+      <c r="J9" s="136">
+        <v>513000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="120" t="s">
+        <v>539</v>
+      </c>
+      <c r="C10" s="132">
+        <v>1590000</v>
+      </c>
+      <c r="D10" s="133">
+        <v>1870000</v>
+      </c>
+      <c r="E10" s="134">
+        <v>1320000</v>
+      </c>
+      <c r="F10" s="134">
+        <v>1550000</v>
+      </c>
+      <c r="G10" s="135">
+        <v>1050000</v>
+      </c>
+      <c r="H10" s="135">
+        <v>1230000</v>
+      </c>
+      <c r="I10" s="136">
+        <v>513000</v>
+      </c>
+      <c r="J10" s="136">
+        <v>598000</v>
+      </c>
+      <c r="O10" s="149" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="120" t="s">
+        <v>540</v>
+      </c>
+      <c r="C11" s="132">
+        <v>1870000</v>
+      </c>
+      <c r="D11" s="137"/>
+      <c r="E11" s="134">
+        <v>1550000</v>
+      </c>
+      <c r="F11" s="138"/>
+      <c r="G11" s="135">
+        <v>1230000</v>
+      </c>
+      <c r="H11" s="139"/>
+      <c r="I11" s="136">
+        <v>598000</v>
+      </c>
+      <c r="J11" s="140"/>
+    </row>
+    <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>527</v>
+      </c>
+      <c r="E14" t="s">
+        <v>528</v>
+      </c>
+      <c r="G14" t="s">
+        <v>529</v>
+      </c>
+      <c r="I14" t="s">
+        <v>530</v>
+      </c>
+      <c r="N14" s="113" t="s">
+        <v>527</v>
+      </c>
+      <c r="O14" s="113" t="s">
+        <v>528</v>
+      </c>
+      <c r="P14" s="113" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q14" s="113" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="115" t="s">
+        <v>533</v>
+      </c>
+      <c r="C15" t="str">
+        <f>C4&amp;" to "&amp;D4</f>
+        <v>0 to 202000</v>
+      </c>
+      <c r="E15" t="str">
+        <f>E4&amp;" to "&amp;F4</f>
+        <v>0 to 174000</v>
+      </c>
+      <c r="G15" t="str">
+        <f>G4&amp;" to "&amp;H4</f>
+        <v>0 to 145000</v>
+      </c>
+      <c r="I15" t="str">
+        <f>I4&amp;" to "&amp;J4</f>
+        <v>0 to 88100</v>
+      </c>
+      <c r="M15" s="115" t="s">
+        <v>573</v>
+      </c>
+      <c r="N15" s="109">
+        <f>O4</f>
+        <v>78600</v>
+      </c>
+      <c r="O15" s="109">
+        <f>Q4</f>
+        <v>63000</v>
+      </c>
+      <c r="P15" s="109">
+        <f>S4</f>
+        <v>47300</v>
+      </c>
+      <c r="Q15" s="109">
+        <f>U4</f>
+        <v>45100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="120" t="s">
+        <v>534</v>
+      </c>
+      <c r="C16" t="str">
+        <f>C5&amp;" to "&amp;D5</f>
+        <v>202000 to 480000</v>
+      </c>
+      <c r="E16" t="str">
+        <f>E5&amp;" to "&amp;F5</f>
+        <v>174000 to 403000</v>
+      </c>
+      <c r="G16" t="str">
+        <f>G5&amp;" to "&amp;H5</f>
+        <v>145000 to 327000</v>
+      </c>
+      <c r="I16" t="str">
+        <f>I5&amp;" to "&amp;J5</f>
+        <v>88100 to 173000</v>
+      </c>
+      <c r="M16" s="120" t="s">
+        <v>574</v>
+      </c>
+      <c r="N16" t="str">
+        <f>O5&amp;" to "&amp;P5</f>
+        <v>6300 to 78600</v>
+      </c>
+      <c r="O16" t="str">
+        <f>Q5&amp;" to "&amp;R5</f>
+        <v>6200 to 63000</v>
+      </c>
+      <c r="P16" t="str">
+        <f>S5&amp;" to "&amp;T5</f>
+        <v>6100 to 47300</v>
+      </c>
+      <c r="Q16" t="str">
+        <f>U5&amp;" to "&amp;V5</f>
+        <v>6000 to 45100</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="120" t="s">
+        <v>535</v>
+      </c>
+      <c r="C17" t="str">
+        <f>C6&amp;" to "&amp;D6</f>
+        <v>480000 to 758000</v>
+      </c>
+      <c r="E17" t="str">
+        <f>E6&amp;" to "&amp;F6</f>
+        <v>403000 to 633000</v>
+      </c>
+      <c r="G17" t="str">
+        <f>G6&amp;" to "&amp;H6</f>
+        <v>327000 to 508000</v>
+      </c>
+      <c r="I17" t="str">
+        <f>I6&amp;" to "&amp;J6</f>
+        <v>173000 to 258000</v>
+      </c>
+      <c r="M17" s="120" t="s">
+        <v>575</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" ref="N17:N18" si="0">O6&amp;" to "&amp;P6</f>
+        <v>1400 to 6300</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" ref="O17:O18" si="1">Q6&amp;" to "&amp;R6</f>
+        <v>1350 to 6200</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" ref="P17:P18" si="2">S6&amp;" to "&amp;T6</f>
+        <v>1300 to 6100</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" ref="Q17:Q18" si="3">U6&amp;" to "&amp;V6</f>
+        <v>1300 to 6000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="120" t="s">
+        <v>536</v>
+      </c>
+      <c r="C18" t="str">
+        <f>C7&amp;" to "&amp;D7</f>
+        <v>758000 to 1040000</v>
+      </c>
+      <c r="E18" t="str">
+        <f>E7&amp;" to "&amp;F7</f>
+        <v>633000 to 863000</v>
+      </c>
+      <c r="G18" t="str">
+        <f>G7&amp;" to "&amp;H7</f>
+        <v>508000 to 690000</v>
+      </c>
+      <c r="I18" t="str">
+        <f>I7&amp;" to "&amp;J7</f>
+        <v>258000 to 343000</v>
+      </c>
+      <c r="M18" s="120" t="s">
+        <v>576</v>
+      </c>
+      <c r="N18" s="109">
+        <f>P7</f>
+        <v>1400</v>
+      </c>
+      <c r="O18" s="109">
+        <f>R7</f>
+        <v>1350</v>
+      </c>
+      <c r="P18" s="109">
+        <f>T7</f>
+        <v>1300</v>
+      </c>
+      <c r="Q18" s="109">
+        <f>V7</f>
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="120" t="s">
+        <v>537</v>
+      </c>
+      <c r="C19" t="str">
+        <f>C8&amp;" to "&amp;D8</f>
+        <v>1040000 to 1310000</v>
+      </c>
+      <c r="E19" t="str">
+        <f>E8&amp;" to "&amp;F8</f>
+        <v>863000 to 1090000</v>
+      </c>
+      <c r="G19" t="str">
+        <f>G8&amp;" to "&amp;H8</f>
+        <v>690000 to 871000</v>
+      </c>
+      <c r="I19" t="str">
+        <f>I8&amp;" to "&amp;J8</f>
+        <v>343000 to 428000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="120" t="s">
+        <v>538</v>
+      </c>
+      <c r="C20" t="str">
+        <f>C9&amp;" to "&amp;D9</f>
+        <v>1310000 to 1590000</v>
+      </c>
+      <c r="E20" t="str">
+        <f>E9&amp;" to "&amp;F9</f>
+        <v>1090000 to 1320000</v>
+      </c>
+      <c r="G20" t="str">
+        <f>G9&amp;" to "&amp;H9</f>
+        <v>871000 to 1050000</v>
+      </c>
+      <c r="I20" t="str">
+        <f>I9&amp;" to "&amp;J9</f>
+        <v>428000 to 513000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="120" t="s">
+        <v>539</v>
+      </c>
+      <c r="C21" t="str">
+        <f>C10&amp;" to "&amp;D10</f>
+        <v>1590000 to 1870000</v>
+      </c>
+      <c r="E21" t="str">
+        <f>E10&amp;" to "&amp;F10</f>
+        <v>1320000 to 1550000</v>
+      </c>
+      <c r="G21" t="str">
+        <f>G10&amp;" to "&amp;H10</f>
+        <v>1050000 to 1230000</v>
+      </c>
+      <c r="I21" t="str">
+        <f>I10&amp;" to "&amp;J10</f>
+        <v>513000 to 598000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="120" t="s">
+        <v>540</v>
+      </c>
+      <c r="C22" t="str">
+        <f>C11&amp;""</f>
+        <v>1870000</v>
+      </c>
+      <c r="E22" t="str">
+        <f>E11&amp;""</f>
+        <v>1550000</v>
+      </c>
+      <c r="G22" t="str">
+        <f>G11&amp;""</f>
+        <v>1230000</v>
+      </c>
+      <c r="I22" t="str">
+        <f>I11&amp;""</f>
+        <v>598000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C25" s="149" t="s">
+        <v>588</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF03E16-6481-44BC-89B4-27A98D72160C}">
+  <dimension ref="B2:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="110" t="s">
+        <v>586</v>
+      </c>
+      <c r="C2" s="110" t="s">
+        <v>527</v>
+      </c>
+      <c r="D2" s="110" t="s">
+        <v>528</v>
+      </c>
+      <c r="E2" s="110" t="s">
+        <v>529</v>
+      </c>
+      <c r="F2" s="110" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="83" t="s">
+        <v>533</v>
+      </c>
+      <c r="C3" t="s">
+        <v>541</v>
+      </c>
+      <c r="D3" t="s">
+        <v>542</v>
+      </c>
+      <c r="E3" t="s">
+        <v>543</v>
+      </c>
+      <c r="F3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="83" t="s">
+        <v>534</v>
+      </c>
+      <c r="C4" t="s">
+        <v>545</v>
+      </c>
+      <c r="D4" t="s">
+        <v>546</v>
+      </c>
+      <c r="E4" t="s">
+        <v>547</v>
+      </c>
+      <c r="F4" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="83" t="s">
+        <v>535</v>
+      </c>
+      <c r="C5" t="s">
+        <v>549</v>
+      </c>
+      <c r="D5" t="s">
+        <v>550</v>
+      </c>
+      <c r="E5" t="s">
+        <v>551</v>
+      </c>
+      <c r="F5" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="83" t="s">
+        <v>536</v>
+      </c>
+      <c r="C6" t="s">
+        <v>553</v>
+      </c>
+      <c r="D6" t="s">
+        <v>554</v>
+      </c>
+      <c r="E6" t="s">
+        <v>555</v>
+      </c>
+      <c r="F6" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="83" t="s">
+        <v>537</v>
+      </c>
+      <c r="C7" t="s">
+        <v>557</v>
+      </c>
+      <c r="D7" t="s">
+        <v>558</v>
+      </c>
+      <c r="E7" t="s">
+        <v>559</v>
+      </c>
+      <c r="F7" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="83" t="s">
+        <v>538</v>
+      </c>
+      <c r="C8" t="s">
+        <v>561</v>
+      </c>
+      <c r="D8" t="s">
+        <v>562</v>
+      </c>
+      <c r="E8" t="s">
+        <v>563</v>
+      </c>
+      <c r="F8" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="83" t="s">
+        <v>539</v>
+      </c>
+      <c r="C9" t="s">
+        <v>565</v>
+      </c>
+      <c r="D9" t="s">
+        <v>566</v>
+      </c>
+      <c r="E9" t="s">
+        <v>567</v>
+      </c>
+      <c r="F9" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="83" t="s">
+        <v>540</v>
+      </c>
+      <c r="C10" t="s">
+        <v>569</v>
+      </c>
+      <c r="D10" t="s">
+        <v>570</v>
+      </c>
+      <c r="E10" t="s">
+        <v>571</v>
+      </c>
+      <c r="F10" t="s">
+        <v>572</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60761244-E2EA-4DCB-98B0-B2653577D4BA}">
+  <dimension ref="B2:F6"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="110" t="s">
+        <v>585</v>
+      </c>
+      <c r="C2" s="110" t="s">
+        <v>527</v>
+      </c>
+      <c r="D2" s="110" t="s">
+        <v>528</v>
+      </c>
+      <c r="E2" s="110" t="s">
+        <v>529</v>
+      </c>
+      <c r="F2" s="110" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="83" t="s">
+        <v>573</v>
+      </c>
+      <c r="C3">
+        <v>78600</v>
+      </c>
+      <c r="D3">
+        <v>63000</v>
+      </c>
+      <c r="E3">
+        <v>47300</v>
+      </c>
+      <c r="F3">
+        <v>45100</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="83" t="s">
+        <v>574</v>
+      </c>
+      <c r="C4" t="s">
+        <v>577</v>
+      </c>
+      <c r="D4" t="s">
+        <v>578</v>
+      </c>
+      <c r="E4" t="s">
+        <v>579</v>
+      </c>
+      <c r="F4" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="83" t="s">
+        <v>575</v>
+      </c>
+      <c r="C5" t="s">
+        <v>581</v>
+      </c>
+      <c r="D5" t="s">
+        <v>582</v>
+      </c>
+      <c r="E5" t="s">
+        <v>583</v>
+      </c>
+      <c r="F5" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="83" t="s">
+        <v>576</v>
+      </c>
+      <c r="C6">
+        <v>1400</v>
+      </c>
+      <c r="D6">
+        <v>1350</v>
+      </c>
+      <c r="E6">
+        <v>1300</v>
+      </c>
+      <c r="F6">
+        <v>1300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>